<commit_message>
je ne sais plus ce que je fais
</commit_message>
<xml_diff>
--- a/TP1.xlsx
+++ b/TP1.xlsx
@@ -5,17 +5,18 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakar\OneDrive\Desktop\Studying v4.0\ADM\TP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\zack_zako\ADM\TP1-Analyse_dm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2AA363-AC94-49E6-B7FF-3FF2A125A8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907FD182-F846-4763-8969-8B347E901D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="401" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="389" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classeur 1" sheetId="1" r:id="rId1"/>
     <sheet name="Classeur 2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil1" sheetId="3" r:id="rId3"/>
+    <sheet name="Feuil2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="137">
   <si>
     <t>Label</t>
   </si>
@@ -474,9 +475,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>Matrice des poids</t>
-  </si>
-  <si>
     <t>Vect 1</t>
   </si>
   <si>
@@ -507,15 +505,40 @@
   <si>
     <t>inertie intra</t>
   </si>
+  <si>
+    <t>Matrice des
+ poids</t>
+  </si>
+  <si>
+    <t>C'WC</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>GG'</t>
+  </si>
+  <si>
+    <t>VAR-COV</t>
+  </si>
+  <si>
+    <t>INERTIE</t>
+  </si>
+  <si>
+    <t>x_i - xhat</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0.0000000_-;\-* #,##0.0000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -1033,18 +1056,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </left>
-      <right style="thin">
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1089,8 +1112,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1115,12 +1139,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1132,18 +1150,31 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="43" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="44" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="45">
     <cellStyle name="20 % - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
@@ -1173,6 +1204,7 @@
     <cellStyle name="Cellule liée" xfId="13" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="10" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Milliers" xfId="44" builtinId="3"/>
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
     <cellStyle name="Neutre" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1500,10 +1532,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:AH256"/>
+  <dimension ref="A1:AH259"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AG27" sqref="AG27"/>
+    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B169" sqref="B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1518,29 +1550,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:32" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
@@ -3696,17 +3728,11 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="AG27">
-        <f>_xlfn.VAR.P(D5:AF25)</f>
-        <v>0.40891217163455595</v>
-      </c>
-    </row>
     <row r="28" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="16"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="2" t="s">
         <v>64</v>
       </c>
@@ -3826,14 +3852,14 @@
         <f t="shared" si="0"/>
         <v>0.17261722902494017</v>
       </c>
-      <c r="AG28" s="25">
+      <c r="AG28" s="22">
         <f>SUM(D28:AF28)</f>
         <v>2.4878107392290194</v>
       </c>
     </row>
     <row r="29" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="2" t="s">
         <v>63</v>
       </c>
@@ -3955,8 +3981,8 @@
       </c>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="2" t="s">
         <v>62</v>
       </c>
@@ -22332,6 +22358,11 @@
       </c>
       <c r="AD256" s="6">
         <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -22351,8 +22382,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:AF106"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B22"/>
+    <sheetView topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31187,10 +31218,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4352CD6-557C-4C33-B75B-903E9CE39D1D}">
-  <dimension ref="A1:AH61"/>
+  <sheetPr codeName="Feuil3"/>
+  <dimension ref="A1:AH39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31220,10 +31252,10 @@
       <c r="G1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="19" cm="1">
+      <c r="K1" s="17" cm="1">
         <f t="array" ref="K1:AE21">(1/21)*_xlfn.MUNIT(21)</f>
         <v>4.7619047619047616E-2</v>
       </c>
@@ -31288,13 +31320,13 @@
         <v>0</v>
       </c>
       <c r="AG1" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AH1" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
@@ -31313,8 +31345,8 @@
         <f t="array" ref="G2:G22">IF(A2:A22="Chinon",1,0)</f>
         <v>0</v>
       </c>
-      <c r="J2" t="s">
-        <v>121</v>
+      <c r="J2" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="K2" s="3">
         <v>0</v>
@@ -32978,52 +33010,55 @@
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="D23" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="E23">
+      <c r="D23" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="25">
         <f>AVERAGE(_xlfn.ANCHORARRAY(E2))</f>
         <v>0.52380952380952384</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="25">
         <f>AVERAGE(_xlfn.ANCHORARRAY(F2))</f>
         <v>0.2857142857142857</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="25">
         <f>AVERAGE(_xlfn.ANCHORARRAY(G2))</f>
         <v>0.19047619047619047</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="E24">
-        <f>VAR(_xlfn.ANCHORARRAY(E2))</f>
-        <v>0.26190476190476192</v>
+        <f>_xlfn.VAR.P(_xlfn.ANCHORARRAY(E2))</f>
+        <v>0.24943310657596371</v>
       </c>
       <c r="F24">
-        <f>VAR(_xlfn.ANCHORARRAY(F2))</f>
-        <v>0.21428571428571427</v>
+        <f t="shared" ref="F24:G24" si="0">_xlfn.VAR.P(_xlfn.ANCHORARRAY(F2))</f>
+        <v>0.20408163265306123</v>
       </c>
       <c r="G24">
-        <f>VAR(_xlfn.ANCHORARRAY(G2))</f>
-        <v>0.16190476190476191</v>
+        <f t="shared" si="0"/>
+        <v>0.15419501133786848</v>
       </c>
     </row>
     <row r="25" spans="1:34" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B25" s="21" t="s">
+      <c r="A25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="E25" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="E25" s="22" t="s">
-        <v>126</v>
-      </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C26" s="20" cm="1">
+      <c r="C26" s="18" cm="1">
         <f t="array" ref="C26:C28">MMULT(TRANSPOSE(E2:G22),MMULT(_xlfn.ANCHORARRAY(K1),AH1:AH21))</f>
         <v>0.52380952380952372</v>
       </c>
@@ -33031,535 +33066,2510 @@
         <f>POWER(C26,2)</f>
         <v>0.27437641723355999</v>
       </c>
-      <c r="G26" cm="1">
-        <f t="array" ref="G26:I28">MMULT(_xlfn.ANCHORARRAY(C26),TRANSPOSE(_xlfn.ANCHORARRAY(C26)))</f>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="B27" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="18">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" ref="E27:E28" si="1">POWER(C27,2)</f>
+        <v>8.1632653061224483E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="B28" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="18">
+        <v>0.19047619047619047</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="1"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D30" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="H30" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="J30" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="K30" s="26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="D31" s="26" cm="1">
+        <f t="array" ref="D31">MMULT(TRANSPOSE(_xlfn.ANCHORARRAY(C26)),E26:E28)</f>
+        <v>0.1739552964042759</v>
+      </c>
+      <c r="E31" s="26">
+        <f>L37+M38+N39</f>
+        <v>0.60770975056689347</v>
+      </c>
+      <c r="F31" s="26">
+        <f>E31+D31</f>
+        <v>0.78166504697116934</v>
+      </c>
+      <c r="H31" s="31">
+        <f>D31/F31</f>
+        <v>0.22254455035225851</v>
+      </c>
+      <c r="J31" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="K31" s="28">
+        <f>G37/B37</f>
+        <v>0.52380952380952372</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="D32" s="21"/>
+      <c r="J32" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K32" s="28">
+        <f>H38/C38</f>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D33" s="21"/>
+      <c r="J33" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="K33" s="28">
+        <f>I39/D39</f>
+        <v>0.19047619047619047</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D34" s="21"/>
+      <c r="K34" s="30">
+        <f>SUM(K31:K33)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F35" s="21"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="3" cm="1">
+        <f t="array" ref="B37:D39">MMULT(MMULT(TRANSPOSE(E2:G22),_xlfn.ANCHORARRAY(K1)),E2:G22)</f>
+        <v>0.52380952380952372</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>133</v>
+      </c>
+      <c r="G37" s="3" cm="1">
+        <f t="array" ref="G37:I39">MMULT(_xlfn.ANCHORARRAY(C26),TRANSPOSE(_xlfn.ANCHORARRAY(C26)))</f>
         <v>0.27437641723355999</v>
       </c>
+      <c r="H37" s="3">
+        <v>0.1496598639455782</v>
+      </c>
+      <c r="I37" s="3">
+        <v>9.9773242630385464E-2</v>
+      </c>
+      <c r="K37" t="s">
+        <v>134</v>
+      </c>
+      <c r="L37" s="3" cm="1">
+        <f t="array" ref="L37:N39">_xlfn.ANCHORARRAY(B37)-_xlfn.ANCHORARRAY(G37)</f>
+        <v>0.24943310657596374</v>
+      </c>
+      <c r="M37" s="3">
+        <v>-0.1496598639455782</v>
+      </c>
+      <c r="N37" s="3">
+        <v>-9.9773242630385464E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B38" s="3">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0.1496598639455782</v>
+      </c>
+      <c r="H38" s="3">
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="I38" s="3">
+        <v>5.4421768707482984E-2</v>
+      </c>
+      <c r="L38" s="3">
+        <v>-0.1496598639455782</v>
+      </c>
+      <c r="M38" s="3">
+        <v>0.20408163265306123</v>
+      </c>
+      <c r="N38" s="3">
+        <v>-5.4421768707482984E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B39" s="3">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.19047619047619047</v>
+      </c>
+      <c r="G39" s="3">
+        <v>9.9773242630385464E-2</v>
+      </c>
+      <c r="H39" s="3">
+        <v>5.4421768707482984E-2</v>
+      </c>
+      <c r="I39" s="3">
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="L39" s="3">
+        <v>-9.9773242630385464E-2</v>
+      </c>
+      <c r="M39" s="3">
+        <v>-5.4421768707482984E-2</v>
+      </c>
+      <c r="N39" s="3">
+        <v>0.15419501133786848</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06125FD9-118D-438F-8796-B7536608E65E}">
+  <dimension ref="B1:AH28"/>
+  <sheetViews>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AB28" sqref="AB28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>B2-$B23</f>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="G2">
+        <f>C2-$C$23</f>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="H2">
+        <f>D2-$D$23</f>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J2">
+        <f>POWER(F2,2)</f>
+        <v>0.22675736961451246</v>
+      </c>
+      <c r="K2">
+        <f>POWER(G2,2)</f>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="L2">
+        <f>POWER(H2,2)</f>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N2" s="17" cm="1">
+        <f t="array" ref="N2:AH22">(1/21)*_xlfn.MUNIT(21)</f>
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>0</v>
+      </c>
+      <c r="R2" s="3">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3">
+        <v>0</v>
+      </c>
+      <c r="T2" s="3">
+        <v>0</v>
+      </c>
+      <c r="U2" s="3">
+        <v>0</v>
+      </c>
+      <c r="V2" s="3">
+        <v>0</v>
+      </c>
+      <c r="W2" s="3">
+        <v>0</v>
+      </c>
+      <c r="X2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F22" si="0">B3-$B$23</f>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G22" si="1">C3-$C$23</f>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H22" si="2">D3-$D$23</f>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J22" si="3">POWER(F3,2)</f>
+        <v>0.22675736961451246</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:L22" si="4">POWER(G3,2)</f>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0</v>
+      </c>
+      <c r="R3" s="3">
+        <v>0</v>
+      </c>
+      <c r="S3" s="3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="3">
+        <v>0</v>
+      </c>
+      <c r="U3" s="3">
+        <v>0</v>
+      </c>
+      <c r="V3" s="3">
+        <v>0</v>
+      </c>
+      <c r="W3" s="3">
+        <v>0</v>
+      </c>
+      <c r="X3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>-0.52380952380952384</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>0.2743764172335601</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="4"/>
+        <v>0.51020408163265307</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0</v>
+      </c>
+      <c r="R4" s="3">
+        <v>0</v>
+      </c>
+      <c r="S4" s="3">
+        <v>0</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0</v>
+      </c>
+      <c r="V4" s="3">
+        <v>0</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0</v>
+      </c>
+      <c r="X4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>-0.52380952380952384</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>0.80952380952380953</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>0.2743764172335601</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="4"/>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>0.65532879818594103</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3">
+        <v>0</v>
+      </c>
+      <c r="T5" s="3">
+        <v>0</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0</v>
+      </c>
+      <c r="X5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>0.22675736961451246</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="4"/>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0</v>
+      </c>
+      <c r="T6" s="3">
+        <v>0</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0</v>
+      </c>
+      <c r="V6" s="3">
+        <v>0</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0</v>
+      </c>
+      <c r="X6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>-0.52380952380952384</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>0.2743764172335601</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="4"/>
+        <v>0.51020408163265307</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0</v>
+      </c>
+      <c r="R7" s="3">
+        <v>0</v>
+      </c>
+      <c r="S7" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="T7" s="3">
+        <v>0</v>
+      </c>
+      <c r="U7" s="3">
+        <v>0</v>
+      </c>
+      <c r="V7" s="3">
+        <v>0</v>
+      </c>
+      <c r="W7" s="3">
+        <v>0</v>
+      </c>
+      <c r="X7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>-0.52380952380952384</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>0.2743764172335601</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="4"/>
+        <v>0.51020408163265307</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3">
+        <v>0</v>
+      </c>
+      <c r="S8" s="3">
+        <v>0</v>
+      </c>
+      <c r="T8" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="U8" s="3">
+        <v>0</v>
+      </c>
+      <c r="V8" s="3">
+        <v>0</v>
+      </c>
+      <c r="W8" s="3">
+        <v>0</v>
+      </c>
+      <c r="X8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>0.22675736961451246</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="4"/>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3">
+        <v>0</v>
+      </c>
+      <c r="S9" s="3">
+        <v>0</v>
+      </c>
+      <c r="T9" s="3">
+        <v>0</v>
+      </c>
+      <c r="U9" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="V9" s="3">
+        <v>0</v>
+      </c>
+      <c r="W9" s="3">
+        <v>0</v>
+      </c>
+      <c r="X9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>-0.52380952380952384</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>0.80952380952380953</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>0.2743764172335601</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="4"/>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="4"/>
+        <v>0.65532879818594103</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>0</v>
+      </c>
+      <c r="R10" s="3">
+        <v>0</v>
+      </c>
+      <c r="S10" s="3">
+        <v>0</v>
+      </c>
+      <c r="T10" s="3">
+        <v>0</v>
+      </c>
+      <c r="U10" s="3">
+        <v>0</v>
+      </c>
+      <c r="V10" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="W10" s="3">
+        <v>0</v>
+      </c>
+      <c r="X10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>0.22675736961451246</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>0</v>
+      </c>
+      <c r="R11" s="3">
+        <v>0</v>
+      </c>
+      <c r="S11" s="3">
+        <v>0</v>
+      </c>
+      <c r="T11" s="3">
+        <v>0</v>
+      </c>
+      <c r="U11" s="3">
+        <v>0</v>
+      </c>
+      <c r="V11" s="3">
+        <v>0</v>
+      </c>
+      <c r="W11" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="X11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>0.22675736961451246</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="4"/>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0</v>
+      </c>
+      <c r="R12" s="3">
+        <v>0</v>
+      </c>
+      <c r="S12" s="3">
+        <v>0</v>
+      </c>
+      <c r="T12" s="3">
+        <v>0</v>
+      </c>
+      <c r="U12" s="3">
+        <v>0</v>
+      </c>
+      <c r="V12" s="3">
+        <v>0</v>
+      </c>
+      <c r="W12" s="3">
+        <v>0</v>
+      </c>
+      <c r="X12" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>0.22675736961451246</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0</v>
+      </c>
+      <c r="O13" s="3">
+        <v>0</v>
+      </c>
+      <c r="P13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>0</v>
+      </c>
+      <c r="R13" s="3">
+        <v>0</v>
+      </c>
+      <c r="S13" s="3">
+        <v>0</v>
+      </c>
+      <c r="T13" s="3">
+        <v>0</v>
+      </c>
+      <c r="U13" s="3">
+        <v>0</v>
+      </c>
+      <c r="V13" s="3">
+        <v>0</v>
+      </c>
+      <c r="W13" s="3">
+        <v>0</v>
+      </c>
+      <c r="X13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>0.22675736961451246</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0</v>
+      </c>
+      <c r="O14" s="3">
+        <v>0</v>
+      </c>
+      <c r="P14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>0</v>
+      </c>
+      <c r="R14" s="3">
+        <v>0</v>
+      </c>
+      <c r="S14" s="3">
+        <v>0</v>
+      </c>
+      <c r="T14" s="3">
+        <v>0</v>
+      </c>
+      <c r="U14" s="3">
+        <v>0</v>
+      </c>
+      <c r="V14" s="3">
+        <v>0</v>
+      </c>
+      <c r="W14" s="3">
+        <v>0</v>
+      </c>
+      <c r="X14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>0.22675736961451246</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0</v>
+      </c>
+      <c r="O15" s="3">
+        <v>0</v>
+      </c>
+      <c r="P15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>0</v>
+      </c>
+      <c r="R15" s="3">
+        <v>0</v>
+      </c>
+      <c r="S15" s="3">
+        <v>0</v>
+      </c>
+      <c r="T15" s="3">
+        <v>0</v>
+      </c>
+      <c r="U15" s="3">
+        <v>0</v>
+      </c>
+      <c r="V15" s="3">
+        <v>0</v>
+      </c>
+      <c r="W15" s="3">
+        <v>0</v>
+      </c>
+      <c r="X15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="AB15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>-0.52380952380952384</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>0.2743764172335601</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>0.51020408163265307</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N16" s="3">
+        <v>0</v>
+      </c>
+      <c r="O16" s="3">
+        <v>0</v>
+      </c>
+      <c r="P16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>0</v>
+      </c>
+      <c r="R16" s="3">
+        <v>0</v>
+      </c>
+      <c r="S16" s="3">
+        <v>0</v>
+      </c>
+      <c r="T16" s="3">
+        <v>0</v>
+      </c>
+      <c r="U16" s="3">
+        <v>0</v>
+      </c>
+      <c r="V16" s="3">
+        <v>0</v>
+      </c>
+      <c r="W16" s="3">
+        <v>0</v>
+      </c>
+      <c r="X16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>-0.52380952380952384</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>0.2743764172335601</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="4"/>
+        <v>0.51020408163265307</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N17" s="3">
+        <v>0</v>
+      </c>
+      <c r="O17" s="3">
+        <v>0</v>
+      </c>
+      <c r="P17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>0</v>
+      </c>
+      <c r="R17" s="3">
+        <v>0</v>
+      </c>
+      <c r="S17" s="3">
+        <v>0</v>
+      </c>
+      <c r="T17" s="3">
+        <v>0</v>
+      </c>
+      <c r="U17" s="3">
+        <v>0</v>
+      </c>
+      <c r="V17" s="3">
+        <v>0</v>
+      </c>
+      <c r="W17" s="3">
+        <v>0</v>
+      </c>
+      <c r="X17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>-0.52380952380952384</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>0.80952380952380953</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>0.2743764172335601</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="4"/>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="4"/>
+        <v>0.65532879818594103</v>
+      </c>
+      <c r="N18" s="3">
+        <v>0</v>
+      </c>
+      <c r="O18" s="3">
+        <v>0</v>
+      </c>
+      <c r="P18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>0</v>
+      </c>
+      <c r="R18" s="3">
+        <v>0</v>
+      </c>
+      <c r="S18" s="3">
+        <v>0</v>
+      </c>
+      <c r="T18" s="3">
+        <v>0</v>
+      </c>
+      <c r="U18" s="3">
+        <v>0</v>
+      </c>
+      <c r="V18" s="3">
+        <v>0</v>
+      </c>
+      <c r="W18" s="3">
+        <v>0</v>
+      </c>
+      <c r="X18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="AE18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>-0.52380952380952384</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>0.80952380952380953</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>0.2743764172335601</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="4"/>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="4"/>
+        <v>0.65532879818594103</v>
+      </c>
+      <c r="N19" s="3">
+        <v>0</v>
+      </c>
+      <c r="O19" s="3">
+        <v>0</v>
+      </c>
+      <c r="P19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>0</v>
+      </c>
+      <c r="R19" s="3">
+        <v>0</v>
+      </c>
+      <c r="S19" s="3">
+        <v>0</v>
+      </c>
+      <c r="T19" s="3">
+        <v>0</v>
+      </c>
+      <c r="U19" s="3">
+        <v>0</v>
+      </c>
+      <c r="V19" s="3">
+        <v>0</v>
+      </c>
+      <c r="W19" s="3">
+        <v>0</v>
+      </c>
+      <c r="X19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="AF19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>-0.52380952380952384</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>0.2743764172335601</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="4"/>
+        <v>0.51020408163265307</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N20" s="3">
+        <v>0</v>
+      </c>
+      <c r="O20" s="3">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>0</v>
+      </c>
+      <c r="R20" s="3">
+        <v>0</v>
+      </c>
+      <c r="S20" s="3">
+        <v>0</v>
+      </c>
+      <c r="T20" s="3">
+        <v>0</v>
+      </c>
+      <c r="U20" s="3">
+        <v>0</v>
+      </c>
+      <c r="V20" s="3">
+        <v>0</v>
+      </c>
+      <c r="W20" s="3">
+        <v>0</v>
+      </c>
+      <c r="X20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="AG20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
+        <v>0.22675736961451246</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="4"/>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N21" s="3">
+        <v>0</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0</v>
+      </c>
+      <c r="P21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>0</v>
+      </c>
+      <c r="R21" s="3">
+        <v>0</v>
+      </c>
+      <c r="S21" s="3">
+        <v>0</v>
+      </c>
+      <c r="T21" s="3">
+        <v>0</v>
+      </c>
+      <c r="U21" s="3">
+        <v>0</v>
+      </c>
+      <c r="V21" s="3">
+        <v>0</v>
+      </c>
+      <c r="W21" s="3">
+        <v>0</v>
+      </c>
+      <c r="X21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="AH21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>-0.19047619047619047</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
+        <v>0.22675736961451246</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="4"/>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="4"/>
+        <v>3.6281179138321989E-2</v>
+      </c>
+      <c r="N22" s="3">
+        <v>0</v>
+      </c>
+      <c r="O22" s="3">
+        <v>0</v>
+      </c>
+      <c r="P22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>0</v>
+      </c>
+      <c r="R22" s="3">
+        <v>0</v>
+      </c>
+      <c r="S22" s="3">
+        <v>0</v>
+      </c>
+      <c r="T22" s="3">
+        <v>0</v>
+      </c>
+      <c r="U22" s="3">
+        <v>0</v>
+      </c>
+      <c r="V22" s="3">
+        <v>0</v>
+      </c>
+      <c r="W22" s="3">
+        <v>0</v>
+      </c>
+      <c r="X22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="3">
+        <v>4.7619047619047616E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <f>AVERAGE(B2:B22)</f>
+        <v>0.52380952380952384</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:D23" si="5">AVERAGE(C2:C22)</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="5"/>
+        <v>0.19047619047619047</v>
+      </c>
+    </row>
+    <row r="25" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="F25" cm="1">
+        <f t="array" ref="F25:Z27">MMULT(TRANSPOSE(J2:L22),_xlfn.ANCHORARRAY(N2))</f>
+        <v>1.079796998164345E-2</v>
+      </c>
+      <c r="G25">
+        <v>1.079796998164345E-2</v>
+      </c>
+      <c r="H25">
+        <v>1.3065543677788576E-2</v>
+      </c>
+      <c r="I25">
+        <v>1.3065543677788576E-2</v>
+      </c>
+      <c r="J25">
+        <v>1.079796998164345E-2</v>
+      </c>
+      <c r="K25">
+        <v>1.3065543677788576E-2</v>
+      </c>
+      <c r="L25">
+        <v>1.3065543677788576E-2</v>
+      </c>
+      <c r="M25">
+        <v>1.079796998164345E-2</v>
+      </c>
+      <c r="N25">
+        <v>1.3065543677788576E-2</v>
+      </c>
+      <c r="O25">
+        <v>1.079796998164345E-2</v>
+      </c>
+      <c r="P25">
+        <v>1.079796998164345E-2</v>
+      </c>
+      <c r="Q25">
+        <v>1.079796998164345E-2</v>
+      </c>
+      <c r="R25">
+        <v>1.079796998164345E-2</v>
+      </c>
+      <c r="S25">
+        <v>1.079796998164345E-2</v>
+      </c>
+      <c r="T25">
+        <v>1.3065543677788576E-2</v>
+      </c>
+      <c r="U25">
+        <v>1.3065543677788576E-2</v>
+      </c>
+      <c r="V25">
+        <v>1.3065543677788576E-2</v>
+      </c>
+      <c r="W25">
+        <v>1.3065543677788576E-2</v>
+      </c>
+      <c r="X25">
+        <v>1.3065543677788576E-2</v>
+      </c>
+      <c r="Y25">
+        <v>1.079796998164345E-2</v>
+      </c>
+      <c r="Z25">
+        <v>1.079796998164345E-2</v>
+      </c>
+      <c r="AB25">
+        <f>SUM(F25:Z25)</f>
+        <v>0.24943310657596376</v>
+      </c>
+    </row>
+    <row r="26" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <v>3.8872691933916417E-3</v>
+      </c>
+      <c r="G26">
+        <v>3.8872691933916417E-3</v>
+      </c>
       <c r="H26">
-        <v>0.1496598639455782</v>
+        <v>2.4295432458697763E-2</v>
       </c>
       <c r="I26">
-        <v>9.9773242630385464E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="B27" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="C27" s="20">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="E27" s="3">
-        <f t="shared" ref="E27:E28" si="0">POWER(C27,2)</f>
-        <v>8.1632653061224483E-2</v>
+        <v>3.8872691933916417E-3</v>
+      </c>
+      <c r="J26">
+        <v>3.8872691933916417E-3</v>
+      </c>
+      <c r="K26">
+        <v>2.4295432458697763E-2</v>
+      </c>
+      <c r="L26">
+        <v>2.4295432458697763E-2</v>
+      </c>
+      <c r="M26">
+        <v>3.8872691933916417E-3</v>
+      </c>
+      <c r="N26">
+        <v>3.8872691933916417E-3</v>
+      </c>
+      <c r="O26">
+        <v>3.8872691933916417E-3</v>
+      </c>
+      <c r="P26">
+        <v>3.8872691933916417E-3</v>
+      </c>
+      <c r="Q26">
+        <v>3.8872691933916417E-3</v>
+      </c>
+      <c r="R26">
+        <v>3.8872691933916417E-3</v>
+      </c>
+      <c r="S26">
+        <v>3.8872691933916417E-3</v>
+      </c>
+      <c r="T26">
+        <v>2.4295432458697763E-2</v>
+      </c>
+      <c r="U26">
+        <v>2.4295432458697763E-2</v>
+      </c>
+      <c r="V26">
+        <v>3.8872691933916417E-3</v>
+      </c>
+      <c r="W26">
+        <v>3.8872691933916417E-3</v>
+      </c>
+      <c r="X26">
+        <v>2.4295432458697763E-2</v>
+      </c>
+      <c r="Y26">
+        <v>3.8872691933916417E-3</v>
+      </c>
+      <c r="Z26">
+        <v>3.8872691933916417E-3</v>
+      </c>
+      <c r="AB26">
+        <f>SUM(F26:Z26)</f>
+        <v>0.20408163265306112</v>
+      </c>
+    </row>
+    <row r="27" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="F27">
+        <v>1.7276751970629518E-3</v>
       </c>
       <c r="G27">
-        <v>0.1496598639455782</v>
+        <v>1.7276751970629518E-3</v>
       </c>
       <c r="H27">
-        <v>8.1632653061224483E-2</v>
+        <v>1.7276751970629518E-3</v>
       </c>
       <c r="I27">
-        <v>5.4421768707482984E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="B28" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="C28" s="20">
-        <v>0.19047619047619047</v>
-      </c>
-      <c r="E28" s="3">
-        <f t="shared" si="0"/>
-        <v>3.6281179138321989E-2</v>
-      </c>
-      <c r="G28">
-        <v>9.9773242630385464E-2</v>
-      </c>
-      <c r="H28">
-        <v>5.4421768707482984E-2</v>
-      </c>
-      <c r="I28">
-        <v>3.6281179138321989E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D30" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="E30" t="s">
-        <v>130</v>
-      </c>
-      <c r="F30" t="s">
-        <v>128</v>
-      </c>
-      <c r="H30" s="26" t="s">
-        <v>129</v>
-      </c>
-      <c r="K30" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="D31" s="3">
-        <f>(C26*E26+C27*E27+C28*E28)</f>
-        <v>0.1739552964042759</v>
-      </c>
-      <c r="E31">
-        <f>SUM(E24:G24)</f>
-        <v>0.63809523809523805</v>
-      </c>
-      <c r="F31">
-        <f>E31+D31</f>
-        <v>0.81205053449951392</v>
-      </c>
-      <c r="H31" s="24">
-        <f>D31/F31</f>
-        <v>0.21421732886548581</v>
-      </c>
-      <c r="J31" t="s">
-        <v>118</v>
-      </c>
-      <c r="K31" s="24">
-        <f>E24/E31</f>
-        <v>0.41044776119402993</v>
-      </c>
-    </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="D32" s="24"/>
-      <c r="J32" t="s">
-        <v>119</v>
-      </c>
-      <c r="K32" s="24">
-        <f>F24/E31</f>
-        <v>0.33582089552238809</v>
-      </c>
-    </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="J33" t="s">
-        <v>120</v>
-      </c>
-      <c r="K33" s="24">
-        <f>G24/E31</f>
-        <v>0.2537313432835821</v>
-      </c>
-    </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D34" s="24"/>
-      <c r="K34" s="27"/>
-    </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="F35" s="24"/>
-    </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C38">
-        <f>E2-$E23</f>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="D38">
-        <f>F2-$F$23</f>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="E38">
-        <f>G2-$G$23</f>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H38">
-        <f>C38/$C$61</f>
-        <v>0.95346258924559246</v>
-      </c>
-    </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C39">
-        <f t="shared" ref="C39:D59" si="1">E3-$E$23</f>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="D39">
-        <f t="shared" ref="D39:D58" si="2">F3-$F$23</f>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="E39">
-        <f t="shared" ref="E39:E58" si="3">G3-$G$23</f>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H39">
-        <f t="shared" ref="H39:H58" si="4">C39/$C$61</f>
-        <v>0.95346258924559246</v>
-      </c>
-    </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C40">
-        <f t="shared" si="1"/>
-        <v>-0.52380952380952384</v>
-      </c>
-      <c r="D40">
-        <f t="shared" si="2"/>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="E40">
-        <f t="shared" si="3"/>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H40">
-        <f t="shared" si="4"/>
-        <v>-1.0488088481701519</v>
-      </c>
-    </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C41">
-        <f t="shared" si="1"/>
-        <v>-0.52380952380952384</v>
-      </c>
-      <c r="D41">
-        <f t="shared" si="2"/>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="E41">
-        <f t="shared" si="3"/>
-        <v>0.80952380952380953</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="4"/>
-        <v>-1.0488088481701519</v>
-      </c>
-    </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C42">
-        <f t="shared" si="1"/>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="D42">
-        <f t="shared" si="2"/>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="E42">
-        <f t="shared" si="3"/>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H42">
-        <f t="shared" si="4"/>
-        <v>0.95346258924559246</v>
-      </c>
-    </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C43">
-        <f t="shared" si="1"/>
-        <v>-0.52380952380952384</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="2"/>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="E43">
-        <f t="shared" si="3"/>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H43">
-        <f t="shared" si="4"/>
-        <v>-1.0488088481701519</v>
-      </c>
-    </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C44">
-        <f t="shared" si="1"/>
-        <v>-0.52380952380952384</v>
-      </c>
-      <c r="D44">
-        <f t="shared" si="2"/>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="E44">
-        <f t="shared" si="3"/>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H44">
-        <f t="shared" si="4"/>
-        <v>-1.0488088481701519</v>
-      </c>
-    </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C45">
-        <f t="shared" si="1"/>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="D45">
-        <f t="shared" si="2"/>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="E45">
-        <f t="shared" si="3"/>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H45">
-        <f t="shared" si="4"/>
-        <v>0.95346258924559246</v>
-      </c>
-    </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C46">
-        <f t="shared" si="1"/>
-        <v>-0.52380952380952384</v>
-      </c>
-      <c r="D46">
-        <f t="shared" si="2"/>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="3"/>
-        <v>0.80952380952380953</v>
-      </c>
-      <c r="H46">
-        <f t="shared" si="4"/>
-        <v>-1.0488088481701519</v>
-      </c>
-    </row>
-    <row r="47" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C47">
-        <f t="shared" si="1"/>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="D47">
-        <f t="shared" si="2"/>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="E47">
-        <f t="shared" si="3"/>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H47">
-        <f t="shared" si="4"/>
-        <v>0.95346258924559246</v>
-      </c>
-    </row>
-    <row r="48" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C48">
-        <f t="shared" si="1"/>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="2"/>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="E48">
-        <f t="shared" si="3"/>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H48">
-        <f t="shared" si="4"/>
-        <v>0.95346258924559246</v>
-      </c>
-    </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C49">
-        <f t="shared" si="1"/>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="D49">
-        <f t="shared" si="2"/>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="E49">
-        <f t="shared" si="3"/>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H49">
-        <f t="shared" si="4"/>
-        <v>0.95346258924559246</v>
-      </c>
-    </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C50">
-        <f t="shared" si="1"/>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="D50">
-        <f t="shared" si="2"/>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="E50">
-        <f t="shared" si="3"/>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H50">
-        <f t="shared" si="4"/>
-        <v>0.95346258924559246</v>
-      </c>
-    </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C51">
-        <f t="shared" si="1"/>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="D51">
-        <f t="shared" si="2"/>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="E51">
-        <f t="shared" si="3"/>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H51">
-        <f t="shared" si="4"/>
-        <v>0.95346258924559246</v>
-      </c>
-    </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C52">
-        <f t="shared" si="1"/>
-        <v>-0.52380952380952384</v>
-      </c>
-      <c r="D52">
-        <f t="shared" si="2"/>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="E52">
-        <f t="shared" si="3"/>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H52">
-        <f t="shared" si="4"/>
-        <v>-1.0488088481701519</v>
-      </c>
-    </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C53">
-        <f t="shared" si="1"/>
-        <v>-0.52380952380952384</v>
-      </c>
-      <c r="D53">
-        <f t="shared" si="2"/>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="E53">
-        <f t="shared" si="3"/>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H53">
-        <f t="shared" si="4"/>
-        <v>-1.0488088481701519</v>
-      </c>
-    </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C54">
-        <f t="shared" si="1"/>
-        <v>-0.52380952380952384</v>
-      </c>
-      <c r="D54">
-        <f t="shared" si="2"/>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="E54">
-        <f t="shared" si="3"/>
-        <v>0.80952380952380953</v>
-      </c>
-      <c r="H54">
-        <f t="shared" si="4"/>
-        <v>-1.0488088481701519</v>
-      </c>
-    </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C55">
-        <f t="shared" si="1"/>
-        <v>-0.52380952380952384</v>
-      </c>
-      <c r="D55">
-        <f t="shared" si="2"/>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="E55">
-        <f t="shared" si="3"/>
-        <v>0.80952380952380953</v>
-      </c>
-      <c r="H55">
-        <f t="shared" si="4"/>
-        <v>-1.0488088481701519</v>
-      </c>
-    </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C56">
-        <f t="shared" si="1"/>
-        <v>-0.52380952380952384</v>
-      </c>
-      <c r="D56">
-        <f t="shared" si="2"/>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="E56">
-        <f t="shared" si="3"/>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H56">
-        <f t="shared" si="4"/>
-        <v>-1.0488088481701519</v>
-      </c>
-    </row>
-    <row r="57" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C57">
-        <f t="shared" si="1"/>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="D57">
-        <f t="shared" si="2"/>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="E57">
-        <f t="shared" si="3"/>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H57">
-        <f t="shared" si="4"/>
-        <v>0.95346258924559246</v>
-      </c>
-    </row>
-    <row r="58" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C58">
-        <f t="shared" si="1"/>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="D58">
-        <f t="shared" si="2"/>
-        <v>-0.2857142857142857</v>
-      </c>
-      <c r="E58">
-        <f t="shared" si="3"/>
-        <v>-0.19047619047619047</v>
-      </c>
-      <c r="H58">
-        <f t="shared" si="4"/>
-        <v>0.95346258924559246</v>
-      </c>
-    </row>
-    <row r="60" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C60">
-        <f>_xlfn.VAR.P(C38:C58)</f>
-        <v>0.24943310657596363</v>
-      </c>
-      <c r="D60">
-        <f t="shared" ref="D60:E60" si="5">_xlfn.VAR.P(D38:D58)</f>
-        <v>0.20408163265306126</v>
-      </c>
-      <c r="E60">
-        <f t="shared" si="5"/>
-        <v>0.1541950113378685</v>
-      </c>
-      <c r="H60">
-        <f>_xlfn.VAR.P(H38:H58)</f>
-        <v>1.0000000000000009</v>
-      </c>
-    </row>
-    <row r="61" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C61">
-        <f>_xlfn.STDEV.P(C38:C58)</f>
-        <v>0.49943278484292919</v>
-      </c>
-      <c r="D61">
-        <f t="shared" ref="D61:E61" si="6">_xlfn.STDEV.P(D38:D58)</f>
-        <v>0.45175395145262565</v>
-      </c>
-      <c r="E61">
-        <f t="shared" si="6"/>
-        <v>0.39267672624930106</v>
+        <v>3.1206133246949572E-2</v>
+      </c>
+      <c r="J27">
+        <v>1.7276751970629518E-3</v>
+      </c>
+      <c r="K27">
+        <v>1.7276751970629518E-3</v>
+      </c>
+      <c r="L27">
+        <v>1.7276751970629518E-3</v>
+      </c>
+      <c r="M27">
+        <v>1.7276751970629518E-3</v>
+      </c>
+      <c r="N27">
+        <v>3.1206133246949572E-2</v>
+      </c>
+      <c r="O27">
+        <v>1.7276751970629518E-3</v>
+      </c>
+      <c r="P27">
+        <v>1.7276751970629518E-3</v>
+      </c>
+      <c r="Q27">
+        <v>1.7276751970629518E-3</v>
+      </c>
+      <c r="R27">
+        <v>1.7276751970629518E-3</v>
+      </c>
+      <c r="S27">
+        <v>1.7276751970629518E-3</v>
+      </c>
+      <c r="T27">
+        <v>1.7276751970629518E-3</v>
+      </c>
+      <c r="U27">
+        <v>1.7276751970629518E-3</v>
+      </c>
+      <c r="V27">
+        <v>3.1206133246949572E-2</v>
+      </c>
+      <c r="W27">
+        <v>3.1206133246949572E-2</v>
+      </c>
+      <c r="X27">
+        <v>1.7276751970629518E-3</v>
+      </c>
+      <c r="Y27">
+        <v>1.7276751970629518E-3</v>
+      </c>
+      <c r="Z27">
+        <v>1.7276751970629518E-3</v>
+      </c>
+      <c r="AB27">
+        <f>SUM(F27:Z27)</f>
+        <v>0.15419501133786848</v>
+      </c>
+    </row>
+    <row r="28" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AB28">
+        <f>SUM(AB25:AB27)</f>
+        <v>0.60770975056689336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>